<commit_message>
Save vacations history with deleted user
</commit_message>
<xml_diff>
--- a/media/download/urlopy.xlsx
+++ b/media/download/urlopy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,138 +470,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alex Admin</t>
+          <t>test3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01-07-2023</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Urlop wypoczynkowy</t>
+          <t>wypoczynkowy</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-01-05</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Alex Admin</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2023-06-28</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>bezpłatny</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2023-07-08</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2023-07-09</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Noll Roman</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2023-06-26</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>wypoczynkowy</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2023-06-26</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2023-07-02</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>6</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tak</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Noll Roman</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2023-06-20</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>wypoczynkowy</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2023-06-20</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2023-06-21</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>Tak</t>
         </is>

</xml_diff>